<commit_message>
use yptu instead of gftfbusx
</commit_message>
<xml_diff>
--- a/results/12-2020/no-addons/fim_noaddons_summary.xlsx
+++ b/results/12-2020/no-addons/fim_noaddons_summary.xlsx
@@ -1,24 +1,82 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malcalakovalski/Documents/GitHub/Fiscal-Impact-Measure/results/12-2020/no-addons/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6002455-C11B-D54A-A8FC-FB72EDB37E4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="18860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>state_health_outlays</t>
+  </si>
+  <si>
+    <t>state_social_benefits</t>
+  </si>
+  <si>
+    <t>state_noncorp_taxes</t>
+  </si>
+  <si>
+    <t>state_corporate_taxes</t>
+  </si>
+  <si>
+    <t>state_subsidies</t>
+  </si>
+  <si>
+    <t>federal_health_outlays</t>
+  </si>
+  <si>
+    <t>federal_social_benefits</t>
+  </si>
+  <si>
+    <t>federal_noncorp_taxes</t>
+  </si>
+  <si>
+    <t>federal_corporate_taxes</t>
+  </si>
+  <si>
+    <t>federal_subsidies</t>
+  </si>
+  <si>
+    <t>federal_cgrants</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +125,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -113,7 +179,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -145,9 +211,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -179,6 +263,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -354,87 +456,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>state_health_outlays</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>state_social_benefits</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>state_noncorp_taxes</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>state_corporate_taxes</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>state_subsidies</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>federal_health_outlays</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>federal_social_benefits</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>federal_noncorp_taxes</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>federal_corporate_taxes</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>federal_subsidies</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>federal_cgrants</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>43921</v>
       </c>
       <c r="B2">
-        <v>200.671</v>
+        <v>200.67099999999999</v>
       </c>
       <c r="C2">
-        <v>186.021</v>
+        <v>186.02099999999999</v>
       </c>
       <c r="D2">
         <v>1862.4</v>
@@ -446,7 +526,7 @@
         <v>0.6</v>
       </c>
       <c r="G2">
-        <v>1228.129</v>
+        <v>1228.1289999999999</v>
       </c>
       <c r="H2">
         <v>1574.779</v>
@@ -461,10 +541,10 @@
         <v>74.5</v>
       </c>
       <c r="L2">
-        <v>204.371</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>204.37100000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44012</v>
       </c>
@@ -472,7 +552,7 @@
         <v>156.16</v>
       </c>
       <c r="C3">
-        <v>370.810666666667</v>
+        <v>370.81066666666698</v>
       </c>
       <c r="D3">
         <v>1779.8</v>
@@ -487,7 +567,7 @@
         <v>1336.74</v>
       </c>
       <c r="H3">
-        <v>3763.789333333334</v>
+        <v>3763.7893333333341</v>
       </c>
       <c r="I3">
         <v>3105.7</v>
@@ -496,21 +576,21 @@
         <v>171.5</v>
       </c>
       <c r="K3">
-        <v>1085.9</v>
+        <v>1085.9000000000001</v>
       </c>
       <c r="L3">
         <v>884.2600000000001</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44104</v>
       </c>
       <c r="B4">
-        <v>197.628</v>
+        <v>197.62799999999999</v>
       </c>
       <c r="C4">
-        <v>143.7329999999999</v>
+        <v>143.73299999999989</v>
       </c>
       <c r="D4">
         <v>1871.3</v>
@@ -522,10 +602,10 @@
         <v>0.6</v>
       </c>
       <c r="G4">
-        <v>1328.772</v>
+        <v>1328.7719999999999</v>
       </c>
       <c r="H4">
-        <v>2653.267</v>
+        <v>2653.2669999999998</v>
       </c>
       <c r="I4">
         <v>3267.5</v>
@@ -534,51 +614,51 @@
         <v>207</v>
       </c>
       <c r="K4">
-        <v>1212.9</v>
+        <v>1212.9000000000001</v>
       </c>
       <c r="L4">
-        <v>242.128</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>242.12799999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44196</v>
       </c>
       <c r="B5">
-        <v>205.169857046954</v>
+        <v>205.16985704695401</v>
       </c>
       <c r="C5">
         <v>119.7103015934359</v>
       </c>
       <c r="D5">
-        <v>1909.140842230012</v>
+        <v>1909.1408422300119</v>
       </c>
       <c r="E5">
-        <v>92.02399613592002</v>
+        <v>92.023996135920015</v>
       </c>
       <c r="F5">
-        <v>0.6019649465167092</v>
+        <v>0.60196494651670918</v>
       </c>
       <c r="G5">
-        <v>1334.531625230035</v>
+        <v>1334.5316252300349</v>
       </c>
       <c r="H5">
-        <v>2317.934366628473</v>
+        <v>2317.9343666284731</v>
       </c>
       <c r="I5">
-        <v>3296.797779813541</v>
+        <v>3296.7977798135412</v>
       </c>
       <c r="J5">
-        <v>217.2155510496505</v>
+        <v>217.21555104965049</v>
       </c>
       <c r="K5">
-        <v>1216.872139383528</v>
+        <v>1216.8721393835281</v>
       </c>
       <c r="L5">
-        <v>229.1307209391703</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>229.13072093917029</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44286</v>
       </c>
@@ -586,54 +666,54 @@
         <v>212.711714093908</v>
       </c>
       <c r="C6">
-        <v>95.69277464312188</v>
+        <v>95.692774643121879</v>
       </c>
       <c r="D6">
-        <v>1940.803777934908</v>
+        <v>1940.8037779349081</v>
       </c>
       <c r="E6">
-        <v>93.55020615065929</v>
+        <v>93.550206150659292</v>
       </c>
       <c r="F6">
-        <v>0.6040046295094899</v>
+        <v>0.60400462950948985</v>
       </c>
       <c r="G6">
-        <v>1340.291250460071</v>
+        <v>1340.2912504600711</v>
       </c>
       <c r="H6">
-        <v>2053.917872188321</v>
+        <v>2053.9178721883209</v>
       </c>
       <c r="I6">
-        <v>3326.095559627083</v>
+        <v>3326.0955596270828</v>
       </c>
       <c r="J6">
-        <v>227.4311020993011</v>
+        <v>227.43110209930111</v>
       </c>
       <c r="K6">
         <v>1220.995358553434</v>
       </c>
       <c r="L6">
-        <v>213.5263477989132</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>213.52634779891321</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44377</v>
       </c>
       <c r="B7">
-        <v>220.2535711408621</v>
+        <v>220.25357114086211</v>
       </c>
       <c r="C7">
-        <v>71.68043207769836</v>
+        <v>71.680432077698356</v>
       </c>
       <c r="D7">
-        <v>1971.665356232323</v>
+        <v>1971.6653562323229</v>
       </c>
       <c r="E7">
-        <v>95.03778930805085</v>
+        <v>95.037789308050847</v>
       </c>
       <c r="F7">
-        <v>0.6061875574147406</v>
+        <v>0.60618755741474062</v>
       </c>
       <c r="G7">
         <v>1346.050875690107</v>
@@ -645,30 +725,30 @@
         <v>3355.393339440624</v>
       </c>
       <c r="J7">
-        <v>237.6466531489517</v>
+        <v>237.64665314895171</v>
       </c>
       <c r="K7">
-        <v>1225.408147313898</v>
+        <v>1225.4081473138981</v>
       </c>
       <c r="L7">
-        <v>198.3564903385607</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>198.35649033856069</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44469</v>
       </c>
       <c r="B8">
-        <v>227.795428187816</v>
+        <v>227.79542818781599</v>
       </c>
       <c r="C8">
-        <v>49.75742254512136</v>
+        <v>49.757422545121358</v>
       </c>
       <c r="D8">
-        <v>2004.651463470501</v>
+        <v>2004.6514634705011</v>
       </c>
       <c r="E8">
-        <v>96.62777855236428</v>
+        <v>96.627778552364276</v>
       </c>
       <c r="F8">
         <v>0.6085448704308245</v>
@@ -680,36 +760,36 @@
         <v>1692.806943814478</v>
       </c>
       <c r="I8">
-        <v>3384.691119254165</v>
+        <v>3384.6911192541652</v>
       </c>
       <c r="J8">
-        <v>247.8622041986023</v>
+        <v>247.86220419860231</v>
       </c>
       <c r="K8">
-        <v>1230.173455575912</v>
+        <v>1230.1734555759119</v>
       </c>
       <c r="L8">
         <v>183.7659871180808</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44561</v>
       </c>
       <c r="B9">
-        <v>225.5280283306597</v>
+        <v>225.52802833065971</v>
       </c>
       <c r="C9">
-        <v>63.88522952843584</v>
+        <v>63.885229528435843</v>
       </c>
       <c r="D9">
-        <v>2026.74470083257</v>
+        <v>2026.7447008325701</v>
       </c>
       <c r="E9">
-        <v>97.69271202645102</v>
+        <v>97.692712026451019</v>
       </c>
       <c r="F9">
-        <v>0.6110859106172505</v>
+        <v>0.61108591061725048</v>
       </c>
       <c r="G9">
         <v>1386.199959089409</v>
@@ -721,7 +801,7 @@
         <v>3433.258874880511</v>
       </c>
       <c r="J9">
-        <v>291.167689117501</v>
+        <v>291.16768911750103</v>
       </c>
       <c r="K9">
         <v>1235.310168312772</v>
@@ -730,7 +810,7 @@
         <v>195.0533202337098</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44651</v>
       </c>
@@ -738,10 +818,10 @@
         <v>223.2606284735034</v>
       </c>
       <c r="C10">
-        <v>80.17042956814157</v>
+        <v>80.170429568141572</v>
       </c>
       <c r="D10">
-        <v>2046.964998207386</v>
+        <v>2046.9649982073861</v>
       </c>
       <c r="E10">
         <v>98.66736645022506</v>
@@ -750,7 +830,7 @@
         <v>0.613723485418602</v>
       </c>
       <c r="G10">
-        <v>1420.589417258676</v>
+        <v>1420.5894172586759</v>
       </c>
       <c r="H10">
         <v>1756.293963726893</v>
@@ -759,54 +839,54 @@
         <v>3481.826630506856</v>
       </c>
       <c r="J10">
-        <v>334.4731740363995</v>
+        <v>334.47317403639948</v>
       </c>
       <c r="K10">
-        <v>1240.642025773704</v>
+        <v>1240.6420257737041</v>
       </c>
       <c r="L10">
         <v>207.1344126604987</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44742</v>
       </c>
       <c r="B11">
-        <v>220.993228616347</v>
+        <v>220.99322861634701</v>
       </c>
       <c r="C11">
-        <v>96.99510127094811</v>
+        <v>96.995101270948112</v>
       </c>
       <c r="D11">
-        <v>2066.980297175637</v>
+        <v>2066.9802971756371</v>
       </c>
       <c r="E11">
-        <v>99.63213958491018</v>
+        <v>99.632139584910178</v>
       </c>
       <c r="F11">
-        <v>0.6164046564976617</v>
+        <v>0.61640465649766174</v>
       </c>
       <c r="G11">
         <v>1454.978875427943</v>
       </c>
       <c r="H11">
-        <v>1755.554020091888</v>
+        <v>1755.5540200918881</v>
       </c>
       <c r="I11">
-        <v>3530.394386133202</v>
+        <v>3530.3943861332018</v>
       </c>
       <c r="J11">
-        <v>377.7786589552982</v>
+        <v>377.77865895529823</v>
       </c>
       <c r="K11">
-        <v>1246.062013110024</v>
+        <v>1246.0620131100241</v>
       </c>
       <c r="L11">
-        <v>219.2973172977977</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>219.29731729779769</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44834</v>
       </c>
@@ -823,28 +903,28 @@
         <v>100.6409293709915</v>
       </c>
       <c r="F12">
-        <v>0.619120081794921</v>
+        <v>0.61912008179492095</v>
       </c>
       <c r="G12">
         <v>1489.36833359721</v>
       </c>
       <c r="H12">
-        <v>1729.631979650156</v>
+        <v>1729.6319796501559</v>
       </c>
       <c r="I12">
-        <v>3578.962141759547</v>
+        <v>3578.9621417595472</v>
       </c>
       <c r="J12">
-        <v>421.0841438741969</v>
+        <v>421.08414387419691</v>
       </c>
       <c r="K12">
         <v>1251.551245348433</v>
       </c>
       <c r="L12">
-        <v>232.1904913366619</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>232.19049133666189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44926</v>
       </c>
@@ -858,13 +938,13 @@
         <v>2109.144742162292</v>
       </c>
       <c r="E13">
-        <v>101.6645410907063</v>
+        <v>101.66454109070629</v>
       </c>
       <c r="F13">
-        <v>0.6218697613103795</v>
+        <v>0.62186976131037952</v>
       </c>
       <c r="G13">
-        <v>1493.579625264793</v>
+        <v>1493.5796252647931</v>
       </c>
       <c r="H13">
         <v>1731.529779708525</v>
@@ -873,42 +953,42 @@
         <v>3625.974592463861</v>
       </c>
       <c r="J13">
-        <v>445.9092484764166</v>
+        <v>445.90924847641662</v>
       </c>
       <c r="K13">
         <v>1257.109722488932</v>
       </c>
       <c r="L13">
-        <v>244.4440181553535</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>244.44401815535349</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>45016</v>
       </c>
       <c r="B14">
-        <v>214.2355356551508</v>
+        <v>214.23553565515081</v>
       </c>
       <c r="C14">
         <v>142.4876637965252</v>
       </c>
       <c r="D14">
-        <v>2130.492530773214</v>
+        <v>2130.4925307732142</v>
       </c>
       <c r="E14">
         <v>102.6935426044696</v>
       </c>
       <c r="F14">
-        <v>0.6246599230837099</v>
+        <v>0.62465992308370988</v>
       </c>
       <c r="G14">
-        <v>1497.790916932376</v>
+        <v>1497.7909169323759</v>
       </c>
       <c r="H14">
         <v>1734.478848120219</v>
       </c>
       <c r="I14">
-        <v>3672.987043168175</v>
+        <v>3672.9870431681752</v>
       </c>
       <c r="J14">
         <v>470.7343530786365</v>
@@ -917,56 +997,56 @@
         <v>1262.75003451372</v>
       </c>
       <c r="L14">
-        <v>257.4425420787031</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>257.44254207870313</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>45107</v>
       </c>
       <c r="B15">
-        <v>211.9903891031308</v>
+        <v>211.99038910313081</v>
       </c>
       <c r="C15">
-        <v>157.9219908217015</v>
+        <v>157.92199082170151</v>
       </c>
       <c r="D15">
-        <v>2150.955098992152</v>
+        <v>2150.9550989921522</v>
       </c>
       <c r="E15">
-        <v>103.6798749153487</v>
+        <v>103.67987491534871</v>
       </c>
       <c r="F15">
-        <v>0.6274625409363856</v>
+        <v>0.62746254093638565</v>
       </c>
       <c r="G15">
         <v>1502.002208599959</v>
       </c>
       <c r="H15">
-        <v>1738.146878041396</v>
+        <v>1738.1468780413959</v>
       </c>
       <c r="I15">
         <v>3719.999493872489</v>
       </c>
       <c r="J15">
-        <v>495.5594576808564</v>
+        <v>495.55945768085638</v>
       </c>
       <c r="K15">
         <v>1268.415526502904</v>
       </c>
       <c r="L15">
-        <v>269.8242367127528</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>269.82423671275279</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>45199</v>
       </c>
       <c r="B16">
-        <v>209.7452425511109</v>
+        <v>209.74524255111089</v>
       </c>
       <c r="C16">
-        <v>173.2853254846975</v>
+        <v>173.28532548469749</v>
       </c>
       <c r="D16">
         <v>2172.880610385213</v>
@@ -975,7 +1055,7 @@
         <v>104.7367236983627</v>
       </c>
       <c r="F16">
-        <v>0.6303056410469334</v>
+        <v>0.63030564104693343</v>
       </c>
       <c r="G16">
         <v>1506.213500267542</v>
@@ -984,27 +1064,27 @@
         <v>1743.874878588342</v>
       </c>
       <c r="I16">
-        <v>3767.011944576803</v>
+        <v>3767.0119445768032</v>
       </c>
       <c r="J16">
-        <v>520.3845622830761</v>
+        <v>520.38456228307609</v>
       </c>
       <c r="K16">
         <v>1274.162853376376</v>
       </c>
       <c r="L16">
-        <v>282.9579189609678</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>282.95791896096779</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>45291</v>
       </c>
       <c r="B17">
-        <v>212.1087554928324</v>
+        <v>212.10875549283239</v>
       </c>
       <c r="C17">
-        <v>172.7758566111596</v>
+        <v>172.77585661115961</v>
       </c>
       <c r="D17">
         <v>2196.054748436442</v>
@@ -1013,19 +1093,19 @@
         <v>105.8537585149185</v>
       </c>
       <c r="F17">
-        <v>0.6331892234153531</v>
+        <v>0.63318922341535311</v>
       </c>
       <c r="G17">
-        <v>1517.683615334627</v>
+        <v>1517.6836153346269</v>
       </c>
       <c r="H17">
-        <v>1761.524043094089</v>
+        <v>1761.5240430940889</v>
       </c>
       <c r="I17">
-        <v>3802.550255742187</v>
+        <v>3802.5502557421869</v>
       </c>
       <c r="J17">
-        <v>533.7069186780396</v>
+        <v>533.70691867803964</v>
       </c>
       <c r="K17">
         <v>1279.992015134136</v>
@@ -1034,7 +1114,7 @@
         <v>284.8440859079293</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>45382</v>
       </c>
@@ -1042,7 +1122,7 @@
         <v>214.4722684345538</v>
       </c>
       <c r="C18">
-        <v>172.6923419107023</v>
+        <v>172.69234191070231</v>
       </c>
       <c r="D18">
         <v>2220.412286380114</v>
@@ -1051,7 +1131,7 @@
         <v>107.0278353184878</v>
       </c>
       <c r="F18">
-        <v>0.6361039459821358</v>
+        <v>0.63610394598213582</v>
       </c>
       <c r="G18">
         <v>1529.153730401712</v>
@@ -1060,7 +1140,7 @@
         <v>1778.481616477271</v>
       </c>
       <c r="I18">
-        <v>3838.088566907572</v>
+        <v>3838.0885669075719</v>
       </c>
       <c r="J18">
         <v>547.0292750730033</v>
@@ -1069,30 +1149,30 @@
         <v>1285.884126802888</v>
       </c>
       <c r="L18">
-        <v>286.8067489078774</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>286.80674890787742</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>45473</v>
       </c>
       <c r="B19">
-        <v>216.8357813762753</v>
+        <v>216.83578137627529</v>
       </c>
       <c r="C19">
         <v>172.999285202235</v>
       </c>
       <c r="D19">
-        <v>2244.341191291877</v>
+        <v>2244.3411912918768</v>
       </c>
       <c r="E19">
-        <v>108.1812512448711</v>
+        <v>108.18125124487111</v>
       </c>
       <c r="F19">
         <v>0.6390248965885913</v>
       </c>
       <c r="G19">
-        <v>1540.623845468796</v>
+        <v>1540.6238454687959</v>
       </c>
       <c r="H19">
         <v>1792.214568108853</v>
@@ -1101,16 +1181,16 @@
         <v>3873.626878072957</v>
       </c>
       <c r="J19">
-        <v>560.3516314679669</v>
+        <v>560.35163146796685</v>
       </c>
       <c r="K19">
-        <v>1291.788828453838</v>
+        <v>1291.7888284538381</v>
       </c>
       <c r="L19">
-        <v>288.81461243302</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>288.81461243301999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>45565</v>
       </c>
@@ -1121,34 +1201,34 @@
         <v>173.8741673912084</v>
       </c>
       <c r="D20">
-        <v>2268.065097797076</v>
+        <v>2268.0650977970759</v>
       </c>
       <c r="E20">
         <v>109.3247858821655</v>
       </c>
       <c r="F20">
-        <v>0.6419614172942282</v>
+        <v>0.64196141729422818</v>
       </c>
       <c r="G20">
-        <v>1552.093960535882</v>
+        <v>1552.0939605358819</v>
       </c>
       <c r="H20">
         <v>1803.970925515257</v>
       </c>
       <c r="I20">
-        <v>3909.16518923834</v>
+        <v>3909.1651892383402</v>
       </c>
       <c r="J20">
         <v>573.6739878629304</v>
       </c>
       <c r="K20">
-        <v>1297.725005060283</v>
+        <v>1297.7250050602829</v>
       </c>
       <c r="L20">
-        <v>290.8798145313602</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>290.87981453136018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>45657</v>
       </c>
@@ -1156,19 +1236,19 @@
         <v>222.1933175719154</v>
       </c>
       <c r="C21">
-        <v>172.6742687666344</v>
+        <v>172.67426876663441</v>
       </c>
       <c r="D21">
-        <v>2292.226955443573</v>
+        <v>2292.2269554435729</v>
       </c>
       <c r="E21">
         <v>110.4894305461498</v>
       </c>
       <c r="F21">
-        <v>0.6449135080990466</v>
+        <v>0.64491350809904657</v>
       </c>
       <c r="G21">
-        <v>1589.161904397305</v>
+        <v>1589.1619043973051</v>
       </c>
       <c r="H21">
         <v>1845.574035042185</v>
@@ -1183,10 +1263,10 @@
         <v>1303.692656622223</v>
       </c>
       <c r="L21">
-        <v>291.4518940223084</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>291.45189402230841</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>45747</v>
       </c>
@@ -1203,7 +1283,7 @@
         <v>111.7102188981396</v>
       </c>
       <c r="F22">
-        <v>0.6478718269435376</v>
+        <v>0.64787182694353762</v>
       </c>
       <c r="G22">
         <v>1626.229848258728</v>
@@ -1212,71 +1292,71 @@
         <v>1880.670991984249</v>
       </c>
       <c r="I22">
-        <v>3988.401986541733</v>
+        <v>3988.4019865417331</v>
       </c>
       <c r="J22">
-        <v>599.2456445212132</v>
+        <v>599.24564452121319</v>
       </c>
       <c r="K22">
-        <v>1309.672898166362</v>
+        <v>1309.6728981663621</v>
       </c>
       <c r="L22">
-        <v>292.7594346162504</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>292.75943461625042</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>45838</v>
       </c>
       <c r="B23">
-        <v>228.1813640797525</v>
+        <v>228.18136407975251</v>
       </c>
       <c r="C23">
-        <v>170.4164562418464</v>
+        <v>170.41645624184639</v>
       </c>
       <c r="D23">
-        <v>2343.178377584353</v>
+        <v>2343.1783775843528</v>
       </c>
       <c r="E23">
         <v>112.9453800342588</v>
       </c>
       <c r="F23">
-        <v>0.6508145756888472</v>
+        <v>0.65081457568884715</v>
       </c>
       <c r="G23">
-        <v>1663.297792120152</v>
+        <v>1663.2977921201521</v>
       </c>
       <c r="H23">
-        <v>1910.004375292176</v>
+        <v>1910.0043752921761</v>
       </c>
       <c r="I23">
         <v>4028.020385193428</v>
       </c>
       <c r="J23">
-        <v>612.0314728503546</v>
+        <v>612.03147285035459</v>
       </c>
       <c r="K23">
         <v>1315.621664755005</v>
       </c>
       <c r="L23">
-        <v>293.3978807089341</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>293.39788070893411</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>45930</v>
       </c>
       <c r="B24">
-        <v>231.175387333671</v>
+        <v>231.17538733367101</v>
       </c>
       <c r="C24">
-        <v>169.7490003336229</v>
+        <v>169.74900033362289</v>
       </c>
       <c r="D24">
-        <v>2369.054767358483</v>
+        <v>2369.0547673584829</v>
       </c>
       <c r="E24">
-        <v>114.1926682069872</v>
+        <v>114.19266820698719</v>
       </c>
       <c r="F24">
         <v>0.6537604384539929</v>
@@ -1288,57 +1368,57 @@
         <v>1932.953941083782</v>
       </c>
       <c r="I24">
-        <v>4067.638783845125</v>
+        <v>4067.6387838451251</v>
       </c>
       <c r="J24">
-        <v>624.817301179496</v>
+        <v>624.81730117949598</v>
       </c>
       <c r="K24">
-        <v>1321.576726334748</v>
+        <v>1321.5767263347479</v>
       </c>
       <c r="L24">
-        <v>294.0780007668992</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>294.07800076689921</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>46022</v>
       </c>
       <c r="B25">
-        <v>234.2909560208819</v>
+        <v>234.29095602088191</v>
       </c>
       <c r="C25">
-        <v>168.9450237981079</v>
+        <v>168.94502379810791</v>
       </c>
       <c r="D25">
-        <v>2395.154791757957</v>
+        <v>2395.1547917579569</v>
       </c>
       <c r="E25">
-        <v>115.4507359678125</v>
+        <v>115.45073596781251</v>
       </c>
       <c r="F25">
-        <v>0.6567063012191389</v>
+        <v>0.65670630121913887</v>
       </c>
       <c r="G25">
-        <v>1728.051869864273</v>
+        <v>1728.0518698642729</v>
       </c>
       <c r="H25">
-        <v>1945.297494348133</v>
+        <v>1945.2974943481329</v>
       </c>
       <c r="I25">
-        <v>4113.66024600366</v>
+        <v>4113.6602460036602</v>
       </c>
       <c r="J25">
-        <v>627.0425659962227</v>
+        <v>627.04256599622272</v>
       </c>
       <c r="K25">
         <v>1327.53178791449</v>
       </c>
       <c r="L25">
-        <v>294.4968006591445</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>294.49680065914453</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>46112</v>
       </c>
@@ -1346,13 +1426,13 @@
         <v>237.406524708093</v>
       </c>
       <c r="C26">
-        <v>168.0345587193225</v>
+        <v>168.03455871932249</v>
       </c>
       <c r="D26">
         <v>2421.469132673386</v>
       </c>
       <c r="E26">
-        <v>116.7191341672309</v>
+        <v>116.71913416723091</v>
       </c>
       <c r="F26">
         <v>0.6596490499644484</v>
@@ -1364,74 +1444,74 @@
         <v>1959.254032082428</v>
       </c>
       <c r="I26">
-        <v>4194.179831033777</v>
+        <v>4194.1798310337772</v>
       </c>
       <c r="J26">
-        <v>629.2678308129495</v>
+        <v>629.26783081294946</v>
       </c>
       <c r="K26">
-        <v>1333.480554503133</v>
+        <v>1333.4805545031329</v>
       </c>
       <c r="L26">
-        <v>295.6513077247375</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>295.65130772473748</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>46203</v>
       </c>
       <c r="B27">
-        <v>240.522093395304</v>
+        <v>240.52209339530401</v>
       </c>
       <c r="C27">
-        <v>167.6565363568878</v>
+        <v>167.65653635688781</v>
       </c>
       <c r="D27">
-        <v>2447.951199557822</v>
+        <v>2447.9511995578218</v>
       </c>
       <c r="E27">
         <v>117.9956170577221</v>
       </c>
       <c r="F27">
-        <v>0.6625793426304126</v>
+        <v>0.66257934263041263</v>
       </c>
       <c r="G27">
-        <v>1783.424137629668</v>
+        <v>1783.4241376296679</v>
       </c>
       <c r="H27">
-        <v>1976.123083872504</v>
+        <v>1976.1230838725039</v>
       </c>
       <c r="I27">
-        <v>4274.699416063894</v>
+        <v>4274.6994160638942</v>
       </c>
       <c r="J27">
-        <v>631.4930956296762</v>
+        <v>631.49309562967619</v>
       </c>
       <c r="K27">
-        <v>1339.40414112738</v>
+        <v>1339.4041411273799</v>
       </c>
       <c r="L27">
         <v>296.1276968693619</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>46295</v>
       </c>
       <c r="B28">
-        <v>243.6376620825149</v>
+        <v>243.63766208251491</v>
       </c>
       <c r="C28">
-        <v>167.4559948999033</v>
+        <v>167.45599489990329</v>
       </c>
       <c r="D28">
-        <v>2474.638264848823</v>
+        <v>2474.6382648488229</v>
       </c>
       <c r="E28">
         <v>119.2819812373022</v>
       </c>
       <c r="F28">
-        <v>0.665500293236868</v>
+        <v>0.66550029323686799</v>
       </c>
       <c r="G28">
         <v>1811.110271512365</v>
@@ -1440,57 +1520,57 @@
         <v>1995.256001116345</v>
       </c>
       <c r="I28">
-        <v>4355.219001094011</v>
+        <v>4355.2190010940112</v>
       </c>
       <c r="J28">
-        <v>633.7183604464029</v>
+        <v>633.71836044640293</v>
       </c>
       <c r="K28">
-        <v>1345.308842778329</v>
+        <v>1345.3088427783291</v>
       </c>
       <c r="L28">
-        <v>297.3374547789164</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>297.33745477891642</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>46387</v>
       </c>
       <c r="B29">
-        <v>246.8738224899409</v>
+        <v>246.87382248994089</v>
       </c>
       <c r="C29">
-        <v>166.9802474902943</v>
+        <v>166.98024749029429</v>
       </c>
       <c r="D29">
-        <v>2501.576919093336</v>
+        <v>2501.5769190933361</v>
       </c>
       <c r="E29">
-        <v>120.5804724534916</v>
+        <v>120.58047245349159</v>
       </c>
       <c r="F29">
-        <v>0.6684305859028324</v>
+        <v>0.66843058590283244</v>
       </c>
       <c r="G29">
-        <v>1840.633107742748</v>
+        <v>1840.6331077427481</v>
       </c>
       <c r="H29">
-        <v>2011.893696146629</v>
+        <v>2011.8936961466291</v>
       </c>
       <c r="I29">
-        <v>4433.276584878554</v>
+        <v>4433.2765848785539</v>
       </c>
       <c r="J29">
-        <v>635.207866727352</v>
+        <v>635.20786672735198</v>
       </c>
       <c r="K29">
-        <v>1351.232429402576</v>
+        <v>1351.2324294025759</v>
       </c>
       <c r="L29">
-        <v>297.5951422320151</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>297.59514223201512</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>46477</v>
       </c>
@@ -1501,34 +1581,34 @@
         <v>166.3980115374151</v>
       </c>
       <c r="D30">
-        <v>2528.776480400749</v>
+        <v>2528.7764804007488</v>
       </c>
       <c r="E30">
-        <v>121.8915398557941</v>
+        <v>121.89153985579409</v>
       </c>
       <c r="F30">
-        <v>0.6713795626878146</v>
+        <v>0.67137956268781462</v>
       </c>
       <c r="G30">
-        <v>1870.155943973131</v>
+        <v>1870.1559439731309</v>
       </c>
       <c r="H30">
         <v>2028.836695249428</v>
       </c>
       <c r="I30">
-        <v>4508.908092471076</v>
+        <v>4508.9080924710761</v>
       </c>
       <c r="J30">
-        <v>636.6973730083012</v>
+        <v>636.69737300830116</v>
       </c>
       <c r="K30">
         <v>1357.193785973418</v>
       </c>
       <c r="L30">
-        <v>297.9155464877823</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>297.91554648778231</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>46568</v>
       </c>
@@ -1536,16 +1616,16 @@
         <v>253.3461433047934</v>
       </c>
       <c r="C31">
-        <v>165.993256489986</v>
+        <v>165.99325648998601</v>
       </c>
       <c r="D31">
-        <v>2556.218312552285</v>
+        <v>2556.2183125522852</v>
       </c>
       <c r="E31">
         <v>123.2142851452017</v>
       </c>
       <c r="F31">
-        <v>0.6743378815323057</v>
+        <v>0.67433788153230567</v>
       </c>
       <c r="G31">
         <v>1899.678780203514</v>
@@ -1554,74 +1634,74 @@
         <v>2044.049055535957</v>
       </c>
       <c r="I31">
-        <v>4584.539600063598</v>
+        <v>4584.5396000635983</v>
       </c>
       <c r="J31">
         <v>638.1868792892501</v>
       </c>
       <c r="K31">
-        <v>1363.174027517557</v>
+        <v>1363.1740275175571</v>
       </c>
       <c r="L31">
-        <v>299.0041410947957</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>299.00414109479573</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>46660</v>
       </c>
       <c r="B32">
-        <v>256.5823037122195</v>
+        <v>256.58230371221953</v>
       </c>
       <c r="C32">
-        <v>165.553005261467</v>
+        <v>165.55300526146701</v>
       </c>
       <c r="D32">
-        <v>2583.986278532447</v>
+        <v>2583.9862785324472</v>
       </c>
       <c r="E32">
         <v>124.5527506672509</v>
       </c>
       <c r="F32">
-        <v>0.6773179985156508</v>
+        <v>0.67731799851565078</v>
       </c>
       <c r="G32">
-        <v>1929.201616433896</v>
+        <v>1929.2016164338961</v>
       </c>
       <c r="H32">
-        <v>2058.808439852786</v>
+        <v>2058.8084398527858</v>
       </c>
       <c r="I32">
-        <v>4660.171107656121</v>
+        <v>4660.1711076561214</v>
       </c>
       <c r="J32">
-        <v>639.6763855701992</v>
+        <v>639.67638557019916</v>
       </c>
       <c r="K32">
         <v>1369.198333999389</v>
       </c>
       <c r="L32">
-        <v>299.4456395844886</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>299.44563958448862</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>46752</v>
       </c>
       <c r="B33">
-        <v>259.940751329776</v>
+        <v>259.94075132977599</v>
       </c>
       <c r="C33">
-        <v>164.7961863009631</v>
+        <v>164.79618630096309</v>
       </c>
       <c r="D33">
-        <v>2611.800835059555</v>
+        <v>2611.8008350595551</v>
       </c>
       <c r="E33">
         <v>125.8934619368202</v>
       </c>
       <c r="F33">
-        <v>0.680329255697359</v>
+        <v>0.68032925569735903</v>
       </c>
       <c r="G33">
         <v>1977.253281348831</v>
@@ -1630,10 +1710,10 @@
         <v>2098.553659222418</v>
       </c>
       <c r="I33">
-        <v>4733.755533010327</v>
+        <v>4733.7555330103269</v>
       </c>
       <c r="J33">
-        <v>645.2966633224106</v>
+        <v>645.29666332241061</v>
       </c>
       <c r="K33">
         <v>1375.285590392212</v>
@@ -1642,15 +1722,15 @@
         <v>300.3913492404522</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>46843</v>
       </c>
       <c r="B34">
-        <v>263.2991989473325</v>
+        <v>263.29919894733251</v>
       </c>
       <c r="C34">
-        <v>164.1813520648193</v>
+        <v>164.18135206481929</v>
       </c>
       <c r="D34">
         <v>2639.056305023304</v>
@@ -1659,45 +1739,45 @@
         <v>127.207224236147</v>
       </c>
       <c r="F34">
-        <v>0.6833560829782488</v>
+        <v>0.68335608297824879</v>
       </c>
       <c r="G34">
         <v>2025.304946263765</v>
       </c>
       <c r="H34">
-        <v>2133.44714496436</v>
+        <v>2133.4471449643602</v>
       </c>
       <c r="I34">
-        <v>4775.374472454258</v>
+        <v>4775.3744724542576</v>
       </c>
       <c r="J34">
-        <v>650.9169410746221</v>
+        <v>650.91694107462206</v>
       </c>
       <c r="K34">
         <v>1381.404321740531</v>
       </c>
       <c r="L34">
-        <v>300.6760753370834</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>300.67607533708338</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>46934</v>
       </c>
       <c r="B35">
-        <v>266.657646564889</v>
+        <v>266.65764656488898</v>
       </c>
       <c r="C35">
-        <v>163.5665178286756</v>
+        <v>163.56651782867559</v>
       </c>
       <c r="D35">
-        <v>2665.575644345298</v>
+        <v>2665.5756443452979</v>
       </c>
       <c r="E35">
-        <v>128.4855037246544</v>
+        <v>128.48550372465439</v>
       </c>
       <c r="F35">
-        <v>0.6864202784971744</v>
+        <v>0.68642027849717435</v>
       </c>
       <c r="G35">
         <v>2073.356611178699</v>
@@ -1715,10 +1795,10 @@
         <v>1387.598592982039</v>
       </c>
       <c r="L35">
-        <v>301.7818731470479</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>301.78187314704792</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>47026</v>
       </c>
@@ -1726,127 +1806,127 @@
         <v>270.0160941824455</v>
       </c>
       <c r="C36">
-        <v>162.9161874114417</v>
+        <v>162.91618741144171</v>
       </c>
       <c r="D36">
-        <v>2691.862030932558</v>
+        <v>2691.8620309325579</v>
       </c>
       <c r="E36">
         <v>129.7525544755606</v>
       </c>
       <c r="F36">
-        <v>0.6895093861747901</v>
+        <v>0.68950938617479007</v>
       </c>
       <c r="G36">
         <v>2121.408276093633</v>
       </c>
       <c r="H36">
-        <v>2190.577573660407</v>
+        <v>2190.5775736604069</v>
       </c>
       <c r="I36">
-        <v>4858.612351342123</v>
+        <v>4858.6123513421226</v>
       </c>
       <c r="J36">
-        <v>662.157496579045</v>
+        <v>662.15749657904496</v>
       </c>
       <c r="K36">
         <v>1393.843224152339</v>
       </c>
       <c r="L36">
-        <v>302.968062993265</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>302.96806299326499</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>47118</v>
       </c>
       <c r="B37">
-        <v>273.5719604069974</v>
+        <v>273.57196040699739</v>
       </c>
       <c r="C37">
-        <v>161.6183775766845</v>
+        <v>161.61837757668451</v>
       </c>
       <c r="D37">
-        <v>2718.148417519818</v>
+        <v>2718.1484175198179</v>
       </c>
       <c r="E37">
-        <v>131.0196052264669</v>
+        <v>131.01960522646689</v>
       </c>
       <c r="F37">
         <v>0.6926234060110964</v>
       </c>
       <c r="G37">
-        <v>2120.165847061976</v>
+        <v>2120.1658470619759</v>
       </c>
       <c r="H37">
-        <v>2163.361106057697</v>
+        <v>2163.3611060576968</v>
       </c>
       <c r="I37">
-        <v>4903.676642187924</v>
+        <v>4903.6766421879238</v>
       </c>
       <c r="J37">
-        <v>666.4204887339998</v>
+        <v>666.42048873399983</v>
       </c>
       <c r="K37">
         <v>1400.138215251432</v>
       </c>
       <c r="L37">
-        <v>303.0125394598555</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>303.01253945985547</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>47208</v>
       </c>
       <c r="B38">
-        <v>277.1278266315493</v>
+        <v>277.12782663154928</v>
       </c>
       <c r="C38">
-        <v>160.320567741927</v>
+        <v>160.32056774192699</v>
       </c>
       <c r="D38">
-        <v>2744.14594271601</v>
+        <v>2744.1459427160098</v>
       </c>
       <c r="E38">
-        <v>132.2727323427478</v>
+        <v>132.27273234274779</v>
       </c>
       <c r="F38">
-        <v>0.6957592239862569</v>
+        <v>0.69575922398625689</v>
       </c>
       <c r="G38">
-        <v>2118.923418030319</v>
+        <v>2118.9234180303192</v>
       </c>
       <c r="H38">
-        <v>2147.650682851897</v>
+        <v>2147.6506828518968</v>
       </c>
       <c r="I38">
-        <v>4950.674823842127</v>
+        <v>4950.6748238421269</v>
       </c>
       <c r="J38">
-        <v>670.6834808889548</v>
+        <v>670.68348088895482</v>
       </c>
       <c r="K38">
-        <v>1406.477271288219</v>
+        <v>1406.4772712882191</v>
       </c>
       <c r="L38">
-        <v>303.8679133707865</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>303.86791337078648</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>47299</v>
       </c>
       <c r="B39">
-        <v>280.6836928561012</v>
+        <v>280.68369285610117</v>
       </c>
       <c r="C39">
         <v>159.0937502693497</v>
       </c>
       <c r="D39">
-        <v>2770.367102537546</v>
+        <v>2770.3671025375461</v>
       </c>
       <c r="E39">
-        <v>133.5366390471258</v>
+        <v>133.53663904712579</v>
       </c>
       <c r="F39">
         <v>0.6989106120605989</v>
@@ -1855,60 +1935,60 @@
         <v>2117.680988998663</v>
       </c>
       <c r="H39">
-        <v>2144.846927132937</v>
+        <v>2144.8469271329368</v>
       </c>
       <c r="I39">
-        <v>4997.673005496329</v>
+        <v>4997.6730054963291</v>
       </c>
       <c r="J39">
-        <v>674.9464730439097</v>
+        <v>674.94647304390969</v>
       </c>
       <c r="K39">
         <v>1412.847802280502</v>
       </c>
       <c r="L39">
-        <v>304.0482893496833</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>304.04828934968327</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>47391</v>
       </c>
       <c r="B40">
-        <v>284.2395590806532</v>
+        <v>284.23955908065318</v>
       </c>
       <c r="C40">
-        <v>157.724948072412</v>
+        <v>157.72494807241199</v>
       </c>
       <c r="D40">
-        <v>2796.755988328088</v>
+        <v>2796.7559883280878</v>
       </c>
       <c r="E40">
-        <v>134.8086304425765</v>
+        <v>134.80863044257649</v>
       </c>
       <c r="F40">
-        <v>0.7020526580754322</v>
+        <v>0.70205265807543216</v>
       </c>
       <c r="G40">
-        <v>2116.438559967006</v>
+        <v>2116.4385599670059</v>
       </c>
       <c r="H40">
-        <v>2154.252842106352</v>
+        <v>2154.2528421063521</v>
       </c>
       <c r="I40">
-        <v>5044.671187150531</v>
+        <v>5044.6711871505313</v>
       </c>
       <c r="J40">
-        <v>679.2094651988645</v>
+        <v>679.20946519886445</v>
       </c>
       <c r="K40">
-        <v>1419.199448299487</v>
+        <v>1419.1994482994869</v>
       </c>
       <c r="L40">
         <v>305.0027227208825</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>47483</v>
       </c>
@@ -1925,95 +2005,95 @@
         <v>136.0891556786041</v>
       </c>
       <c r="F41">
-        <v>0.7051947040902652</v>
+        <v>0.70519470409026519</v>
       </c>
       <c r="G41">
-        <v>2165.42361822453</v>
+        <v>2165.4236182245299</v>
       </c>
       <c r="H41">
-        <v>2221.525875455438</v>
+        <v>2221.5258754554379</v>
       </c>
       <c r="I41">
-        <v>5091.578997060215</v>
+        <v>5091.5789970602154</v>
       </c>
       <c r="J41">
-        <v>683.2646820013754</v>
+        <v>683.26468200137538</v>
       </c>
       <c r="K41">
         <v>1425.551094318472</v>
       </c>
       <c r="L41">
-        <v>305.202246550351</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>305.20224655035099</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>47573</v>
       </c>
       <c r="B42">
-        <v>292.0032074021328</v>
+        <v>292.00320740213277</v>
       </c>
       <c r="C42">
-        <v>152.8740058679153</v>
+        <v>152.87400586791529</v>
       </c>
       <c r="D42">
         <v>2850.120800800702</v>
       </c>
       <c r="E42">
-        <v>137.3809096522328</v>
+        <v>137.38090965223279</v>
       </c>
       <c r="F42">
-        <v>0.7083367501050983</v>
+        <v>0.70833675010509833</v>
       </c>
       <c r="G42">
         <v>2214.408676482054</v>
       </c>
       <c r="H42">
-        <v>2278.407505250257</v>
+        <v>2278.4075052502571</v>
       </c>
       <c r="I42">
-        <v>5138.292239444817</v>
+        <v>5138.2922394448169</v>
       </c>
       <c r="J42">
-        <v>687.3198988038864</v>
+        <v>687.31989880388642</v>
       </c>
       <c r="K42">
-        <v>1431.902740337457</v>
+        <v>1431.9027403374571</v>
       </c>
       <c r="L42">
         <v>304.6947757516308</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>47664</v>
       </c>
       <c r="B43">
-        <v>295.8850315628728</v>
+        <v>295.88503156287283</v>
       </c>
       <c r="C43">
         <v>150.3420462223971</v>
       </c>
       <c r="D43">
-        <v>2877.068773154603</v>
+        <v>2877.0687731546032</v>
       </c>
       <c r="E43">
         <v>138.6798500179261</v>
       </c>
       <c r="F43">
-        <v>0.7114694540604224</v>
+        <v>0.71146945406042239</v>
       </c>
       <c r="G43">
         <v>2263.393734739579</v>
       </c>
       <c r="H43">
-        <v>2319.479494032694</v>
+        <v>2319.4794940326942</v>
       </c>
       <c r="I43">
-        <v>5185.005481829418</v>
+        <v>5185.0054818294184</v>
       </c>
       <c r="J43">
-        <v>691.3751156063975</v>
+        <v>691.37511560639746</v>
       </c>
       <c r="K43">
         <v>1438.235501383145</v>
@@ -2022,59 +2102,59 @@
         <v>304.9710702947599</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>47756</v>
       </c>
       <c r="B44">
-        <v>299.7668557236126</v>
+        <v>299.76685572361259</v>
       </c>
       <c r="C44">
-        <v>147.8810789390589</v>
+        <v>147.88107893905891</v>
       </c>
       <c r="D44">
-        <v>2904.156517149345</v>
+        <v>2904.1565171493448</v>
       </c>
       <c r="E44">
         <v>139.9855276261801</v>
       </c>
       <c r="F44">
-        <v>0.7145865879165652</v>
+        <v>0.71458658791656515</v>
       </c>
       <c r="G44">
-        <v>2312.378792997103</v>
+        <v>2312.3787929971031</v>
       </c>
       <c r="H44">
-        <v>2347.944425713181</v>
+        <v>2347.9444257131809</v>
       </c>
       <c r="I44">
-        <v>5231.718724214022</v>
+        <v>5231.7187242140217</v>
       </c>
       <c r="J44">
-        <v>695.4303324089084</v>
+        <v>695.43033240890838</v>
       </c>
       <c r="K44">
-        <v>1444.536787473338</v>
+        <v>1444.5367874733381</v>
       </c>
       <c r="L44">
-        <v>305.2714196614735</v>
-      </c>
-    </row>
-    <row r="45">
+        <v>305.27141966147349</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>47848</v>
       </c>
       <c r="D45">
-        <v>2931.402669003705</v>
+        <v>2931.4026690037049</v>
       </c>
       <c r="E45">
-        <v>141.2988407760028</v>
+        <v>141.29884077600281</v>
       </c>
       <c r="F45">
-        <v>0.7176943797131988</v>
+        <v>0.71769437971319883</v>
       </c>
       <c r="K45">
-        <v>1450.819188590233</v>
+        <v>1450.8191885902329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>